<commit_message>
Creating account with nickname and knee elements descritpions update
</commit_message>
<xml_diff>
--- a/Assets/Resources/CSV/LearnKneeLocalization.xlsx
+++ b/Assets/Resources/CSV/LearnKneeLocalization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdude\OneDrive\Pulpit\Unity\Konrad_Dudek-Praca_Magisterska\Assets\Resources\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8B6F35-079D-4CA8-94EF-229EB13D9446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CF232D-5904-4778-A299-CA391883C258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8D4D4752-D6F4-4947-96F6-AEAAB4AF41A2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Element Name</t>
   </si>
@@ -44,24 +44,109 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Rzepka</t>
-  </si>
-  <si>
-    <t>Opis</t>
-  </si>
-  <si>
     <t>Kość Udowa</t>
   </si>
   <si>
-    <t>Opis kości udowej</t>
+    <t>Więzadło rzepki</t>
+  </si>
+  <si>
+    <t>Miejsce przyczepu końcowego mięśnia czworogłowego uda pomiędzy rzepką a guzowatością kości piszczelowej</t>
+  </si>
+  <si>
+    <t>Więzadło krzyżowe przednie</t>
+  </si>
+  <si>
+    <t>Przebiega od powierzchni przyśrodkowej kłykcia bocznego kości udowej przednio-przyśrodkowo do pola międzykłykciowego przedniego kości piszczelowej</t>
+  </si>
+  <si>
+    <t>Więzadło krzyżowe tylne</t>
+  </si>
+  <si>
+    <t>Przebiega od powierzchni przyśrodkowej kłykcia przyśrodkowego do dołu, do pola międzykłykciowego tylnego</t>
+  </si>
+  <si>
+    <t>Więzadło poprzeczne</t>
+  </si>
+  <si>
+    <t>Łączy dwie łękotki od przodu, nie jest pokryte błoną maziową (jedyne prawdziwe więzadło śródstawowe ciała ludzkiego)</t>
+  </si>
+  <si>
+    <t>Łąkotka przyśrodkowa</t>
+  </si>
+  <si>
+    <t>Półkolista, w kształcie litery C
+Przyczepia się do pola międzykłykciowego przedniego i tylnego
+Mocno przytwierdzona przyśrodkowo do torebki stawowej, a bocznie - do więzadła pobocznego piszczelowego, które ogranicza jej ruchomość</t>
+  </si>
+  <si>
+    <t>Łąkotka boczna</t>
+  </si>
+  <si>
+    <t>Prawie całkowicie kolista
+Przyczpia się do pola międzykłykciowego przedniego i tylnego
+Nie jest przytwierdzona do torebki stawowej, więc jest bardziej ruchoma od łąkotki przyśrodkowej</t>
+  </si>
+  <si>
+    <t>Jest trzeszczką znajdującą się w mięśnia czworogłowego uda. Jest elementem składowym stawu kolanowgo</t>
+  </si>
+  <si>
+    <t>Kość piszczelowa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jest kością o funkcji strukturalnej, tworzącą podudzie. Należy do kości długich. Koniec dalszy kości piszczelowej tworzy kostkę przyśrodkową. </t>
+  </si>
+  <si>
+    <t>To najdłuższa kość ciała ludzkiego. Pokrywa ją gruba warstwa mieśni i w związku z tym jedynie jej niewielki fragment jest dostępny badaniu palpacyjnemu</t>
+  </si>
+  <si>
+    <t>Kłykieć przyśrodkowy</t>
+  </si>
+  <si>
+    <t>Kłykieć boczny</t>
+  </si>
+  <si>
+    <t>Kość strzałkowa</t>
+  </si>
+  <si>
+    <t>Staw piszczelowy</t>
+  </si>
+  <si>
+    <t>Rzepka kolanowa</t>
+  </si>
+  <si>
+    <t>Staw rzepkowy</t>
+  </si>
+  <si>
+    <t>Staw strzałkowy</t>
+  </si>
+  <si>
+    <t>Więzadło poboczne strzałkowe</t>
+  </si>
+  <si>
+    <t>Więzadło poboczne piszczelowe</t>
+  </si>
+  <si>
+    <t>Rozpościera się od przyśrodkowej powierzchni kości udowej aż do przyśrodkowej powierzchni piszczeli, stąd odpowiada za stabilność stawu kolanowego od strony przyśrodkowej (czyli od wewnątrz).</t>
+  </si>
+  <si>
+    <t>Rozpościera się od bocznej powierzchni kości udowej aż do tzw. głowy kości strzałkowej i odpowiada za stabilność kolana od strony bocznej</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -90,8 +175,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -406,43 +503,146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42FA13F9-4EBF-46CA-BDCD-3827A8DF10DF}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed sounds and added new descritpions
</commit_message>
<xml_diff>
--- a/Assets/Resources/CSV/LearnKneeLocalization.xlsx
+++ b/Assets/Resources/CSV/LearnKneeLocalization.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdude\OneDrive\Pulpit\Unity\Konrad_Dudek-Praca_Magisterska\Assets\Resources\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8AE6CF-7164-4972-B4F9-C6AB3254145C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB4AADD-A71C-42AB-AD54-045444625216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8D4D4752-D6F4-4947-96F6-AEAAB4AF41A2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="LearnKneeLocalization" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Element Name</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Kość Udowa</t>
-  </si>
-  <si>
     <t>Więzadło rzepki</t>
   </si>
   <si>
@@ -65,19 +62,9 @@
     <t>Łąkotka przyśrodkowa</t>
   </si>
   <si>
-    <t>Półkolista, w kształcie litery C
-Przyczepia się do pola międzykłykciowego przedniego i tylnego
-Mocno przytwierdzona przyśrodkowo do torebki stawowej, a bocznie - do więzadła pobocznego piszczelowego, które ogranicza jej ruchomość</t>
-  </si>
-  <si>
     <t>Łąkotka boczna</t>
   </si>
   <si>
-    <t>Prawie całkowicie kolista
-Przyczpia się do pola międzykłykciowego przedniego i tylnego
-Nie jest przytwierdzona do torebki stawowej, więc jest bardziej ruchoma od łąkotki przyśrodkowej</t>
-  </si>
-  <si>
     <t>Kość piszczelowa</t>
   </si>
   <si>
@@ -105,18 +92,9 @@
     <t>Rozpościera się od bocznej powierzchni kości udowej aż do tzw. głowy kości strzałkowej i odpowiada za stabilność kolana od strony bocznej</t>
   </si>
   <si>
-    <t>Jest to kość spłaszczona trójkątna z zaaokgąglonymi brzegami, włączona w ścięgno mięśnia czworogłowego uda i położona od dolnego końca kości udowej.</t>
-  </si>
-  <si>
     <t>Powierzchnia stawowa rzepki</t>
   </si>
   <si>
-    <t>Czyli tylna, powyżej wierzchołka pokryta jest grubą warstwą chrząstki szklistej; dzieli się ona na dwa pola, z których pole boczne jest większe od przyśrodkowego; obie te części przedzielone są podłużnie biegnącym wzniesieniem. Odpowiada ono podłużnemu rowkowi na powierzchni rzepkowej kości udowej.</t>
-  </si>
-  <si>
-    <t>Więzadło rzepki łączy ją z kością piszczelową; w ruchach zgięcia i prostowania stawu kolanowego rzepka porusza się razem z kością piszczelową. W przypadku wyprostowanego kolana i napiętych mięśni prostujących część dolna powierzchni stawowej rzepki spoczywa na powierzchni rzepkowej kości udowej, część górna leży powyżej; gdy kolano jest zgięte, rzepka przesuwa się ku dołowi i do tyłu, układa się w rowku między obu kłykciami kości udowej i jest unieruchomiona. Gdy kolano jest wyprostowane i mięśnie rozkurczone, rzepka może być przesuwana na boki. Poniżej powierzchni stawowej znajduje się wypukłe chropowate pole, którego dolna część służy za przyczep więzadła rzepki.</t>
-  </si>
-  <si>
     <t xml:space="preserve">To najdłuższa kość ciała ludzkiego. Jak każda kość długa składa się z trzonu i dwóch końców. Na powierzchni tylnej trzonu zaznacza się wydatna kresa chropowa (linea aspera), złożona z dwóch warg, przyśrodkowej (labium mediale) i bocznej (labium laterale). Ku dołowi obie wargi rozchodząc się ograniczają powierzchnię podkolanową (facies poplitea). Warga przyśrodkowa kończy się u dołu guzkiem przywodziciela (tuberculum adductorium). </t>
   </si>
   <si>
@@ -133,6 +111,39 @@
   </si>
   <si>
     <t>Więzadło poprzeczne kolana rozpięte jest między najbardziej do przodu położonymi punktami obu łąkotek, łącząc je. Jest to więzadło cienkie, okrągławe, często powstrzymane w rozwoju. Nieraz może go całkowicie brakować. Napina się ono podczas ruchów obrotowych stawu na zewnątrz.</t>
+  </si>
+  <si>
+    <t>Więzadło łąkotkowo-udowe tylne</t>
+  </si>
+  <si>
+    <t>Płaska powierzchnia stawowa strzałkowa zlokalizowana jest na kłykciu bocznym kości piszczelowej. Powierzchnia stawowa strzałkowa skierowana jest ku dołowi, ku tyłowi i bocznie i przylega do powierzchni stawowej głowy strzałki.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kłykieć przyśrodkowy stawu kolanowego, zwany również guzkiem przyśrodkowym lub wyrostkiem przyśrodkowym, to ważna struktura anatomiczna w obrębie stawu kolanowego. Jest to wyrostek kostny znajdujący się na wewnętrznej stronie kości udowej, blisko stawu kolanowego. Kłykieć przyśrodkowy jest kluczowy dla stabilności i funkcji stawu kolanowego </t>
+  </si>
+  <si>
+    <t>Powierzchnia stawowa kości piszczelowej jest wklęsła i przylega do odpowiedniej powierzchni stawowej kości udowej. Kształt tej powierzchni jest asymetryczny, co pozwala na pewne ograniczenia w ruchomości stawu kolanowego, chroniąc go przed nadmiernymi skręceniami.</t>
+  </si>
+  <si>
+    <t>Więzadło przyczepia się w okolicy tylnego przyczepu łąkotki bocznej. Biegnie ku górze i przyśrodkowo do tyłu od więzadła krzyżowego tylnego. Przeważnie łączy się z nim kończąc się w miejscu jego przyczepu do wewnętrznej powierzchni kłykcia przyśrodkowego kości udowej.</t>
+  </si>
+  <si>
+    <t>Kość udowa</t>
+  </si>
+  <si>
+    <t>Jest to kość spłaszczona trójkątna z zaokrąglonymi brzegami, włączona w ścięgno mięśnia czworogłowego uda i położona od dolnego końca kości udowej.</t>
+  </si>
+  <si>
+    <t>Więzadło rzepki łączy ją z kością piszczelową w ruchach zgięcia i prostowania stawu kolanowego rzepka porusza się razem z kością piszczelową. W przypadku wyprostowanego kolana i napiętych mięśni prostujących część dolna powierzchni stawowej rzepki spoczywa na powierzchni rzepkowej kości udowej, część górna leży powyżej; gdy kolano jest zgięte, rzepka przesuwa się ku dołowi i do tyłu, układa się w rowku między obu kłykciami kości udowej i jest unieruchomiona. Gdy kolano jest wyprostowane i mięśnie rozkurczone, rzepka może być przesuwana na boki. Poniżej powierzchni stawowej znajduje się wypukłe chropowate pole, którego dolna część służy za przyczep więzadła rzepki.</t>
+  </si>
+  <si>
+    <t>Czyli tylna, powyżej wierzchołka pokryta jest grubą warstwą chrząstki szklistej dzieli się ona na dwa pola, z których pole boczne jest większe od przyśrodkowego obie te części przedzielone są podłużnie biegnącym wzniesieniem. Odpowiada ono podłużnemu rowkowi na powierzchni rzepkowej kości udowej.</t>
+  </si>
+  <si>
+    <t>Półkolista, w kształcie litery C.  Przyczepia się do pola międzykłykciowego przedniego i tylnego. Mocno przytwierdzona przyśrodkowo do torebki stawowej, a bocznie - do więzadła pobocznego piszczelowego, które ogranicza jej ruchomość</t>
+  </si>
+  <si>
+    <t>Prawie całkowicie kolista. Przyczpia się do pola międzykłykciowego przedniego i tylnego. Nie jest przytwierdzona do torebki stawowej, więc jest bardziej ruchoma od łąkotki przyśrodkowej</t>
   </si>
 </sst>
 </file>
@@ -508,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42FA13F9-4EBF-46CA-BDCD-3827A8DF10DF}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="128" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -528,126 +539,138 @@
     </row>
     <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>28</v>
+      <c r="B16" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Achievement fixes, added quiz descriptions, latin language fix, deselect element after answer in selection quiz
</commit_message>
<xml_diff>
--- a/Assets/Resources/CSV/LearnKneeLocalization.xlsx
+++ b/Assets/Resources/CSV/LearnKneeLocalization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdude\OneDrive\Pulpit\Unity\Konrad_Dudek-Praca_Magisterska\Assets\Resources\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB4AADD-A71C-42AB-AD54-045444625216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A087AD9-87F6-42D6-A43F-F1F018D3EADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8D4D4752-D6F4-4947-96F6-AEAAB4AF41A2}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="20376" windowHeight="12216" xr2:uid="{8D4D4752-D6F4-4947-96F6-AEAAB4AF41A2}"/>
   </bookViews>
   <sheets>
     <sheet name="LearnKneeLocalization" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Element Name</t>
   </si>
@@ -143,7 +143,58 @@
     <t>Półkolista, w kształcie litery C.  Przyczepia się do pola międzykłykciowego przedniego i tylnego. Mocno przytwierdzona przyśrodkowo do torebki stawowej, a bocznie - do więzadła pobocznego piszczelowego, które ogranicza jej ruchomość</t>
   </si>
   <si>
-    <t>Prawie całkowicie kolista. Przyczpia się do pola międzykłykciowego przedniego i tylnego. Nie jest przytwierdzona do torebki stawowej, więc jest bardziej ruchoma od łąkotki przyśrodkowej</t>
+    <t>It is a flattened triangular bone with rounded edges, incorporated into the quadriceps tendon and located at the lower end of the femur.</t>
+  </si>
+  <si>
+    <t>It is a bone with a structural function that forms the lower leg. It belongs to long bones. The distal end of the tibia forms the medial malleolus.</t>
+  </si>
+  <si>
+    <t>It is the longest bone in the human body. Like any long bone, it consists of a shaft and two ends. On the back surface of the body there is a prominent rough line (linea aspera), composed of two lips: the medial one (labium mediale) and the lateral one (labium laterale). Downwards, both lips spread apart and limit the popliteal surface (facies poplitea). The medial lip ends at the bottom with the adductor tubercle (tuberculum adductorium).</t>
+  </si>
+  <si>
+    <t>The patellar ligament connects it to the tibia. During the flexion and extension movements of the knee joint, the patella moves together with the tibia. When the knee is straight and the extensor muscles are tense, the lower part of the articular surface of the patella rests on the patella surface of the femur, the upper part lies above it; when the knee is bent, the patella moves down and back, lies in the groove between the two condyles of the femur and is immobilized. When the knee is straight and the muscles are relaxed, the patella can be moved sideways. Below the articular surface there is a convex rough area, the lower part of which serves as an attachment for the patellar ligament.</t>
+  </si>
+  <si>
+    <t>It runs from the medial surface of the lateral condyle of the femur anteromedial to the anterior intercondylar area of the tibia.</t>
+  </si>
+  <si>
+    <t>It runs from the medial surface of the medial condyle down to the posterior intercondylar area of the tibia.</t>
+  </si>
+  <si>
+    <t>The transverse knee ligament spans between the most forward points of both menisci, connecting them. It is a thin, round ligament, often inhibited in development. Sometimes it may be completely missing. It tightens when the joint rotates outwards.</t>
+  </si>
+  <si>
+    <t>Semicircular, C-shaped. Attached to the anterior and posterior intercondylar area. Firmly attached medially to the joint capsule, and laterally - to the tibial collateral ligament, which limits its mobility</t>
+  </si>
+  <si>
+    <t>Prawie całkowicie kolista. Przyczepia się do pola międzykłykciowego przedniego i tylnego. Nie jest przytwierdzona do torebki stawowej, więc jest bardziej ruchoma od łąkotki przyśrodkowej</t>
+  </si>
+  <si>
+    <t>Almost completely circular. It attaches to the anterior and posterior intercondylar areas. It is not attached to the joint capsule, so it is more mobile than the medial meniscus</t>
+  </si>
+  <si>
+    <t>The medial condyle of the knee, also called the medial tubercle or medial process, is an important anatomical structure within the knee joint. This is a bony protrusion located on the inside of the femur, close to the knee joint. The medial condyle is crucial to the stability and function of the knee joint</t>
+  </si>
+  <si>
+    <t>It is located on the medial side of the shin and is the longest bone of the skeleton after the femur. It has a triangular shape in cross-section. At the top, where it is involved in the formation of the knee joint, the bone thickens significantly, tapers downwards, and then widens again, although to a lesser extent than at the top. Like any long bone, it consists of a shaft and two ends</t>
+  </si>
+  <si>
+    <t>The articular surface of the tibia is concave and adheres to the corresponding articular surface of the femur. The shape of this surface is asymmetrical, which allows for certain limitations in the mobility of the knee joint, protecting it against excessive twisting.</t>
+  </si>
+  <si>
+    <t>That is, the posterior one, above the apex, is covered with a thick layer of hyaline cartilage. It is divided into two fields, the lateral field of which is larger than the medial one, both of these parts are divided by a longitudinally running hill. It corresponds to a longitudinal groove on the patella surface of the femur.</t>
+  </si>
+  <si>
+    <t>The flat sagittal articular surface is located on the lateral condyle of the tibia. The articular surface of the fibula is directed downwards, posteriorly and laterally and is adjacent to the articular surface of the head of the fibula.</t>
+  </si>
+  <si>
+    <t>It extends from the lateral surface of the femur to the so-called the head of the fibula and is responsible for the stability of the knee from the lateral side</t>
+  </si>
+  <si>
+    <t>It extends from the medial surface of the femur to the medial surface of the tibia, hence it is responsible for the stability of the knee joint from the medial side (i.e. from the inside).</t>
+  </si>
+  <si>
+    <t>The ligament attaches near the posterior attachment of the lateral meniscus. It runs upwards and medially posteriorly from the posterior cruciate ligament. It usually joins it, ending at its attachment to the inner surface of the medial condyle of the femur.</t>
   </si>
 </sst>
 </file>
@@ -517,19 +568,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42FA13F9-4EBF-46CA-BDCD-3827A8DF10DF}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="128" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="52.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -537,140 +589,191 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="C4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C5" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C6" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="C7" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C14" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="C17" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>